<commit_message>
load CAFR2017 demographic data
</commit_message>
<xml_diff>
--- a/Inputs_data/RawMaterials/2017 CAFR Statistics converted by Nuance.xlsx
+++ b/Inputs_data/RawMaterials/2017 CAFR Statistics converted by Nuance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\RSF_NYCTRS\Inputs_data\RawMaterials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABC0F6C2-86D5-479C-B4F2-1C4C36801769}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FA415B4-38BD-4C41-A8A3-B52EB5E3A6BF}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" firstSheet="1" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="16" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="694">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="695">
   <si>
     <r>
       <rPr>
@@ -10829,6 +10829,9 @@
   </si>
   <si>
     <t>STATISTICAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -13247,7 +13250,7 @@
   <dimension ref="A6:F57"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14004,8 +14007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="J46" sqref="J46"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14474,7 +14477,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A4:I56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
@@ -15179,7 +15182,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -15857,7 +15862,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -16108,6 +16115,9 @@
       <c r="A20" s="90" t="s">
         <v>586</v>
       </c>
+      <c r="H20" t="s">
+        <v>694</v>
+      </c>
     </row>
     <row r="22" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
@@ -16653,7 +16663,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -17769,7 +17781,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
@@ -18861,8 +18873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L58"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55:L55"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19539,7 +19551,7 @@
   <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20057,7 +20069,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A3:K55"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
@@ -20919,7 +20931,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:N49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
@@ -22155,7 +22167,7 @@
   <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
have a internally consistent model in k = -1 sim
</commit_message>
<xml_diff>
--- a/Inputs_data/RawMaterials/2017 CAFR Statistics converted by Nuance.xlsx
+++ b/Inputs_data/RawMaterials/2017 CAFR Statistics converted by Nuance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\RSF_NYCTRS\Inputs_data\RawMaterials\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\RSF_NYCTRS\Inputs_data\RawMaterials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FA415B4-38BD-4C41-A8A3-B52EB5E3A6BF}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{95C3C8C6-119B-495C-89DA-41B25B76F35D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" firstSheet="1" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="16" r:id="rId1"/>
@@ -30,7 +30,7 @@
     <sheet name="Sheet14" sheetId="14" r:id="rId15"/>
     <sheet name="Sheet15" sheetId="15" r:id="rId16"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
@@ -11225,7 +11225,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="425">
+  <cellXfs count="426">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -12493,6 +12493,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -13249,7 +13250,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A6:F57"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
@@ -16663,8 +16664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22164,10 +22165,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22178,6 +22179,7 @@
     <col min="4" max="4" width="12.140625" customWidth="1"/>
     <col min="5" max="5" width="15.5703125" customWidth="1"/>
     <col min="6" max="6" width="16.85546875" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -22253,7 +22255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="235" t="s">
         <v>321</v>
       </c>
@@ -22273,7 +22275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="235" t="s">
         <v>323</v>
       </c>
@@ -22293,7 +22295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="235" t="s">
         <v>325</v>
       </c>
@@ -22313,7 +22315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="235" t="s">
         <v>327</v>
       </c>
@@ -22333,7 +22335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="235" t="s">
         <v>329</v>
       </c>
@@ -22353,7 +22355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="235" t="s">
         <v>331</v>
       </c>
@@ -22373,7 +22375,7 @@
         <v>50492</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="235" t="s">
         <v>333</v>
       </c>
@@ -22393,7 +22395,7 @@
         <v>48560</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="235" t="s">
         <v>335</v>
       </c>
@@ -22413,7 +22415,7 @@
         <v>52426</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="235" t="s">
         <v>337</v>
       </c>
@@ -22433,7 +22435,7 @@
         <v>47297</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="235" t="s">
         <v>339</v>
       </c>
@@ -22453,7 +22455,7 @@
         <v>41378</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="235" t="s">
         <v>341</v>
       </c>
@@ -22473,7 +22475,7 @@
         <v>37275</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="235" t="s">
         <v>343</v>
       </c>
@@ -22493,7 +22495,7 @@
         <v>36601</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="240" t="s">
         <v>345</v>
       </c>
@@ -22513,7 +22515,7 @@
         <v>32755</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="220"/>
       <c r="B30" s="220"/>
       <c r="C30" s="220"/>
@@ -22521,7 +22523,7 @@
       <c r="E30" s="220"/>
       <c r="F30" s="220"/>
     </row>
-    <row r="31" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="243" t="s">
         <v>347</v>
       </c>
@@ -22539,6 +22541,10 @@
       </c>
       <c r="F31" s="245">
         <v>45535</v>
+      </c>
+      <c r="H31" s="425">
+        <f>B31*C31+E31*F31</f>
+        <v>3721781548</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>